<commit_message>
changing header in portfolio file
</commit_message>
<xml_diff>
--- a/yes-genie-testautomation-GenieDataCreation/src/main/resources/portfolio.xlsx
+++ b/yes-genie-testautomation-GenieDataCreation/src/main/resources/portfolio.xlsx
@@ -153,7 +153,7 @@
     <t xml:space="preserve">I</t>
   </si>
   <si>
-    <t xml:space="preserve">DEPOSIT</t>
+    <t xml:space="preserve">DEPOSITS</t>
   </si>
   <si>
     <t xml:space="preserve">YES</t>
@@ -168,7 +168,7 @@
     <t xml:space="preserve">FD</t>
   </si>
   <si>
-    <t xml:space="preserve">Fixed Deposit</t>
+    <t xml:space="preserve">Fixed DEPOSITS</t>
   </si>
   <si>
     <t xml:space="preserve">Stagnant</t>
@@ -192,7 +192,7 @@
     <t xml:space="preserve">RD</t>
   </si>
   <si>
-    <t xml:space="preserve">Recurring Deposit Account</t>
+    <t xml:space="preserve">Recurring DEPOSITS Account</t>
   </si>
   <si>
     <t xml:space="preserve">996264849_DA</t>
@@ -482,11 +482,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D\-MMM\-YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -509,12 +510,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -588,7 +583,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -625,10 +620,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -637,7 +628,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Normal" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -715,23 +706,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.8673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="38.9030612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.2091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2091836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.5051020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.969387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.3826530612245"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="48.5357142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="98.7857142857143"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.25"/>
-    <col collapsed="false" hidden="false" max="257" min="16" style="1" width="11.484693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.484693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="38.3367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="47.9234693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="97.5969387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="257" min="16" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,24 +893,24 @@
   </sheetPr>
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.9234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.6275510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="16.6479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.2397959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.0612244897959"/>
-    <col collapsed="false" hidden="false" max="257" min="12" style="1" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.70918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="257" min="12" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2521,12 +2512,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="31.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.9234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="22.2295918367347"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="7" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="7" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2603,7 +2594,7 @@
       <c r="A6" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="4" t="n">
         <v>998003452</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2617,7 +2608,7 @@
       <c r="A7" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="4" t="n">
         <v>998003452</v>
       </c>
       <c r="C7" s="3" t="s">

</xml_diff>